<commit_message>
ActorLevelPackTable 의 skillId 컬럼명을 levelPackId 로 변경
</commit_message>
<xml_diff>
--- a/Excel/LevelPack.xlsx
+++ b/Excel/LevelPack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3997BA4-3471-4458-8C47-3CEC0566F5EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6C1FA9-755B-47EA-BCA5-AAFD47EB92BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3414120-1328-4246-945C-5504AE9FCCB0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D3414120-1328-4246-945C-5504AE9FCCB0}"/>
   </bookViews>
   <sheets>
     <sheet name="LevelPackTable" sheetId="2" r:id="rId1"/>
@@ -88,10 +88,11 @@
     <t>actorId|String</t>
   </si>
   <si>
-    <t>skillId|String</t>
-  </si>
-  <si>
     <t>overridingMax|Int</t>
+  </si>
+  <si>
+    <t>levelPackId|String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -460,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A689B08-E54F-4986-989E-FC7EE88EA9D3}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -531,7 +532,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527A07CA-0D0F-4615-B8C2-37C34C75AD21}">
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -705,12 +706,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387DAB05-D72F-4D4F-B706-92DD4D47ED58}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -719,10 +720,10 @@
         <v>17</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
LevelPack.xlsx 안에 StageExpTable 올림
</commit_message>
<xml_diff>
--- a/Excel/LevelPack.xlsx
+++ b/Excel/LevelPack.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C18B87-7A4F-416B-88A6-7F3C1B4FC4DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD83BE64-98FD-4FBB-A6DA-B0C2B38E58C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3414120-1328-4246-945C-5504AE9FCCB0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3414120-1328-4246-945C-5504AE9FCCB0}"/>
   </bookViews>
   <sheets>
-    <sheet name="LevelPackTable" sheetId="2" r:id="rId1"/>
-    <sheet name="LevelPackLevelTable" sheetId="3" r:id="rId2"/>
-    <sheet name="ActorLevelPackTable" sheetId="4" r:id="rId3"/>
+    <sheet name="StageExpTable" sheetId="5" r:id="rId1"/>
+    <sheet name="LevelPackTable" sheetId="2" r:id="rId2"/>
+    <sheet name="LevelPackLevelTable" sheetId="3" r:id="rId3"/>
+    <sheet name="ActorLevelPackTable" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Skill_ActiveOne001_Name</t>
   </si>
@@ -93,6 +94,21 @@
   <si>
     <t>levelPackId|String</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requiredExp|Int</t>
+  </si>
+  <si>
+    <t>requiredAccumulatedExp|Int</t>
+  </si>
+  <si>
+    <t>exclusive|Bool</t>
+  </si>
+  <si>
+    <t>dropWeight|Float</t>
+  </si>
+  <si>
+    <t>useActor|String!</t>
   </si>
 </sst>
 </file>
@@ -458,10 +474,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7688E9-6191-474A-BC61-D0CBD7110CAB}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A689B08-E54F-4986-989E-FC7EE88EA9D3}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -471,14 +677,15 @@
   <cols>
     <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="25.75" customWidth="1"/>
-    <col min="5" max="5" width="30.75" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="3" max="4" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="25.75" customWidth="1"/>
+    <col min="7" max="7" width="30.75" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -486,38 +693,53 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="G2" t="b">
+      <c r="I2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -527,7 +749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527A07CA-0D0F-4615-B8C2-37C34C75AD21}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -699,7 +921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387DAB05-D72F-4D4F-B706-92DD4D47ED58}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
icon 컬럼명을 iconAddress 로 변경
</commit_message>
<xml_diff>
--- a/Excel/LevelPack.xlsx
+++ b/Excel/LevelPack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69615731-22B1-4B44-890E-E7DCFF51A050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB8A563-2626-4B35-9FCA-EED6BB183ADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D3414120-1328-4246-945C-5504AE9FCCB0}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>levelPackId|String</t>
   </si>
   <si>
-    <t>icon|String</t>
-  </si>
-  <si>
     <t>affectorValueId|String!</t>
   </si>
   <si>
@@ -822,6 +819,9 @@
   </si>
   <si>
     <t>LevelPackUIDesc_MineOnMove</t>
+  </si>
+  <si>
+    <t>iconAddress|String</t>
   </si>
 </sst>
 </file>
@@ -1196,13 +1196,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1405,42 +1405,42 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -1449,13 +1449,13 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H2">
         <v>9</v>
@@ -1466,25 +1466,25 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>69</v>
       </c>
       <c r="H3">
         <v>9</v>
@@ -1493,30 +1493,30 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>74</v>
-      </c>
-      <c r="G4" t="s">
-        <v>75</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -1530,10 +1530,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1542,13 +1542,13 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" t="s">
         <v>78</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
       </c>
       <c r="H5">
         <v>9</v>
@@ -1559,25 +1559,25 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>81</v>
       </c>
-      <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>82</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>83</v>
-      </c>
-      <c r="G6" t="s">
-        <v>84</v>
       </c>
       <c r="H6">
         <v>9</v>
@@ -1586,30 +1586,30 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>87</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>88</v>
-      </c>
-      <c r="G7" t="s">
-        <v>89</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1620,10 +1620,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
         <v>90</v>
-      </c>
-      <c r="B8" t="s">
-        <v>91</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -1632,13 +1632,13 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
         <v>92</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>94</v>
       </c>
       <c r="H8">
         <v>6</v>
@@ -1649,25 +1649,25 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>95</v>
       </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>96</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>97</v>
-      </c>
-      <c r="G9" t="s">
-        <v>98</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -1678,25 +1678,25 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
         <v>99</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>100</v>
       </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>101</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>102</v>
-      </c>
-      <c r="G10" t="s">
-        <v>103</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1707,10 +1707,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
         <v>104</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -1719,13 +1719,13 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" t="s">
         <v>106</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>107</v>
-      </c>
-      <c r="G11" t="s">
-        <v>108</v>
       </c>
       <c r="H11">
         <v>9</v>
@@ -1736,25 +1736,25 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>109</v>
       </c>
-      <c r="B12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>110</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>111</v>
-      </c>
-      <c r="G12" t="s">
-        <v>112</v>
       </c>
       <c r="H12">
         <v>9</v>
@@ -1765,25 +1765,25 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
         <v>113</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>114</v>
       </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>115</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>116</v>
-      </c>
-      <c r="G13" t="s">
-        <v>117</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -1794,10 +1794,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" t="s">
         <v>118</v>
-      </c>
-      <c r="B14" t="s">
-        <v>119</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1806,13 +1806,13 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
         <v>120</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>121</v>
-      </c>
-      <c r="G14" t="s">
-        <v>122</v>
       </c>
       <c r="H14">
         <v>9</v>
@@ -1823,10 +1823,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" t="s">
         <v>123</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1835,13 +1835,13 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" t="s">
         <v>125</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>126</v>
-      </c>
-      <c r="G15" t="s">
-        <v>127</v>
       </c>
       <c r="H15">
         <v>9</v>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -1864,13 +1864,13 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>18</v>
-      </c>
-      <c r="G16" t="s">
-        <v>19</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1893,13 +1893,13 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
         <v>21</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>23</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1910,10 +1910,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1922,13 +1922,13 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>26</v>
-      </c>
-      <c r="G18" t="s">
-        <v>27</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1939,25 +1939,25 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>29</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -1968,25 +1968,25 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>33</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>34</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
       </c>
       <c r="H20">
         <v>2</v>
@@ -1997,25 +1997,25 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>37</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>38</v>
-      </c>
-      <c r="G21" t="s">
-        <v>39</v>
       </c>
       <c r="H21">
         <v>2</v>
@@ -2026,25 +2026,25 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>41</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>42</v>
-      </c>
-      <c r="G22" t="s">
-        <v>43</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -2055,25 +2055,25 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>45</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>46</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -2084,25 +2084,25 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>48</v>
       </c>
-      <c r="B24" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>49</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>50</v>
-      </c>
-      <c r="G24" t="s">
-        <v>51</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -2113,25 +2113,25 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>52</v>
       </c>
-      <c r="B25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>53</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>54</v>
-      </c>
-      <c r="G25" t="s">
-        <v>55</v>
       </c>
       <c r="H25">
         <v>2</v>
@@ -2142,25 +2142,25 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>56</v>
       </c>
-      <c r="B26" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>57</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>58</v>
-      </c>
-      <c r="G26" t="s">
-        <v>59</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
         <v>139</v>
-      </c>
-      <c r="B27" t="s">
-        <v>140</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -2183,13 +2183,13 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
+        <v>140</v>
+      </c>
+      <c r="F27" t="s">
         <v>141</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>142</v>
-      </c>
-      <c r="G27" t="s">
-        <v>143</v>
       </c>
       <c r="H27">
         <v>2</v>
@@ -2200,25 +2200,25 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
         <v>144</v>
       </c>
-      <c r="B28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>145</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>146</v>
-      </c>
-      <c r="G28" t="s">
-        <v>147</v>
       </c>
       <c r="H28">
         <v>2</v>
@@ -2229,10 +2229,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
         <v>152</v>
-      </c>
-      <c r="B29" t="s">
-        <v>153</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -2241,13 +2241,13 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F29" t="s">
+        <v>153</v>
+      </c>
+      <c r="G29" t="s">
         <v>154</v>
-      </c>
-      <c r="G29" t="s">
-        <v>155</v>
       </c>
       <c r="H29">
         <v>9</v>
@@ -2256,30 +2256,30 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>230</v>
+      </c>
+      <c r="F30" t="s">
         <v>156</v>
       </c>
-      <c r="B30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>231</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>157</v>
-      </c>
-      <c r="G30" t="s">
-        <v>158</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -2288,15 +2288,15 @@
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" t="s">
         <v>159</v>
-      </c>
-      <c r="B31" t="s">
-        <v>160</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -2305,13 +2305,13 @@
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F31" t="s">
+        <v>160</v>
+      </c>
+      <c r="G31" t="s">
         <v>161</v>
-      </c>
-      <c r="G31" t="s">
-        <v>162</v>
       </c>
       <c r="H31">
         <v>5</v>
@@ -2322,25 +2322,25 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>232</v>
+      </c>
+      <c r="F32" t="s">
         <v>163</v>
       </c>
-      <c r="B32" t="s">
-        <v>160</v>
-      </c>
-      <c r="C32" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>233</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>164</v>
-      </c>
-      <c r="G32" t="s">
-        <v>165</v>
       </c>
       <c r="H32">
         <v>5</v>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" t="s">
         <v>166</v>
-      </c>
-      <c r="B33" t="s">
-        <v>167</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -2363,13 +2363,13 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F33" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" t="s">
         <v>168</v>
-      </c>
-      <c r="G33" t="s">
-        <v>169</v>
       </c>
       <c r="H33">
         <v>9</v>
@@ -2380,10 +2380,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" t="s">
         <v>170</v>
-      </c>
-      <c r="B34" t="s">
-        <v>171</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -2392,13 +2392,13 @@
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F34" t="s">
+        <v>171</v>
+      </c>
+      <c r="G34" t="s">
         <v>172</v>
-      </c>
-      <c r="G34" t="s">
-        <v>173</v>
       </c>
       <c r="H34">
         <v>5</v>
@@ -2409,25 +2409,25 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>235</v>
+      </c>
+      <c r="F35" t="s">
         <v>174</v>
       </c>
-      <c r="B35" t="s">
-        <v>171</v>
-      </c>
-      <c r="C35" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>236</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>175</v>
-      </c>
-      <c r="G35" t="s">
-        <v>176</v>
       </c>
       <c r="H35">
         <v>5</v>
@@ -2438,10 +2438,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" t="s">
         <v>177</v>
-      </c>
-      <c r="B36" t="s">
-        <v>178</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -2450,13 +2450,13 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F36" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" t="s">
         <v>179</v>
-      </c>
-      <c r="G36" t="s">
-        <v>180</v>
       </c>
       <c r="H36">
         <v>5</v>
@@ -2467,25 +2467,25 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>237</v>
+      </c>
+      <c r="F37" t="s">
         <v>181</v>
       </c>
-      <c r="B37" t="s">
-        <v>178</v>
-      </c>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>238</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>182</v>
-      </c>
-      <c r="G37" t="s">
-        <v>183</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -2496,10 +2496,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
         <v>184</v>
-      </c>
-      <c r="B38" t="s">
-        <v>185</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -2508,13 +2508,13 @@
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F38" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" t="s">
         <v>186</v>
-      </c>
-      <c r="G38" t="s">
-        <v>187</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -2525,25 +2525,25 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F39" t="s">
         <v>188</v>
       </c>
-      <c r="B39" t="s">
-        <v>185</v>
-      </c>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>240</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>189</v>
-      </c>
-      <c r="G39" t="s">
-        <v>190</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2554,10 +2554,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" t="s">
         <v>191</v>
-      </c>
-      <c r="B40" t="s">
-        <v>192</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -2566,13 +2566,13 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G40" t="s">
         <v>193</v>
-      </c>
-      <c r="G40" t="s">
-        <v>194</v>
       </c>
       <c r="H40">
         <v>9</v>
@@ -2583,25 +2583,25 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" t="s">
+        <v>191</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>241</v>
+      </c>
+      <c r="F41" t="s">
         <v>195</v>
       </c>
-      <c r="B41" t="s">
-        <v>192</v>
-      </c>
-      <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>242</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>196</v>
-      </c>
-      <c r="G41" t="s">
-        <v>197</v>
       </c>
       <c r="H41">
         <v>5</v>
@@ -2612,10 +2612,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" t="s">
         <v>198</v>
-      </c>
-      <c r="B42" t="s">
-        <v>199</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -2624,13 +2624,13 @@
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F42" t="s">
+        <v>199</v>
+      </c>
+      <c r="G42" t="s">
         <v>200</v>
-      </c>
-      <c r="G42" t="s">
-        <v>201</v>
       </c>
       <c r="H42">
         <v>9</v>
@@ -2641,25 +2641,25 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
+        <v>198</v>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>243</v>
+      </c>
+      <c r="F43" t="s">
         <v>202</v>
       </c>
-      <c r="B43" t="s">
-        <v>199</v>
-      </c>
-      <c r="C43" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>244</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>203</v>
-      </c>
-      <c r="G43" t="s">
-        <v>204</v>
       </c>
       <c r="H43">
         <v>5</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" t="s">
         <v>148</v>
-      </c>
-      <c r="B44" t="s">
-        <v>149</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -2682,13 +2682,13 @@
         <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F44" t="s">
+        <v>149</v>
+      </c>
+      <c r="G44" t="s">
         <v>150</v>
-      </c>
-      <c r="G44" t="s">
-        <v>151</v>
       </c>
       <c r="H44">
         <v>6</v>
@@ -2697,15 +2697,15 @@
         <v>0</v>
       </c>
       <c r="K44" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>204</v>
+      </c>
+      <c r="B45" t="s">
         <v>205</v>
-      </c>
-      <c r="B45" t="s">
-        <v>206</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -2714,13 +2714,13 @@
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F45" t="s">
+        <v>206</v>
+      </c>
+      <c r="G45" t="s">
         <v>207</v>
-      </c>
-      <c r="G45" t="s">
-        <v>208</v>
       </c>
       <c r="H45">
         <v>6</v>
@@ -2729,15 +2729,15 @@
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -2746,13 +2746,13 @@
         <v>7</v>
       </c>
       <c r="E46" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" t="s">
         <v>260</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>261</v>
-      </c>
-      <c r="G46" t="s">
-        <v>262</v>
       </c>
       <c r="H46">
         <v>6</v>
@@ -2761,15 +2761,15 @@
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" t="s">
         <v>225</v>
-      </c>
-      <c r="B47" t="s">
-        <v>226</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -2778,13 +2778,13 @@
         <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F47" t="s">
+        <v>226</v>
+      </c>
+      <c r="G47" t="s">
         <v>227</v>
-      </c>
-      <c r="G47" t="s">
-        <v>228</v>
       </c>
       <c r="H47">
         <v>5</v>
@@ -2795,10 +2795,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" t="s">
         <v>209</v>
-      </c>
-      <c r="B48" t="s">
-        <v>210</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -2807,16 +2807,16 @@
         <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F48" t="s">
+        <v>210</v>
+      </c>
+      <c r="G48" t="s">
         <v>211</v>
       </c>
-      <c r="G48" t="s">
-        <v>212</v>
-      </c>
       <c r="H48">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2824,10 +2824,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" t="s">
         <v>213</v>
-      </c>
-      <c r="B49" t="s">
-        <v>214</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -2836,13 +2836,13 @@
         <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F49" t="s">
+        <v>214</v>
+      </c>
+      <c r="G49" t="s">
         <v>215</v>
-      </c>
-      <c r="G49" t="s">
-        <v>216</v>
       </c>
       <c r="H49">
         <v>5</v>
@@ -2851,15 +2851,15 @@
         <v>0</v>
       </c>
       <c r="K49" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>216</v>
+      </c>
+      <c r="B50" t="s">
         <v>217</v>
-      </c>
-      <c r="B50" t="s">
-        <v>218</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -2868,30 +2868,30 @@
         <v>7</v>
       </c>
       <c r="E50" t="s">
+        <v>249</v>
+      </c>
+      <c r="F50" t="s">
+        <v>218</v>
+      </c>
+      <c r="G50" t="s">
+        <v>219</v>
+      </c>
+      <c r="H50">
+        <v>9</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="s">
         <v>250</v>
-      </c>
-      <c r="F50" t="s">
-        <v>219</v>
-      </c>
-      <c r="G50" t="s">
-        <v>220</v>
-      </c>
-      <c r="H50">
-        <v>5</v>
-      </c>
-      <c r="I50" t="b">
-        <v>0</v>
-      </c>
-      <c r="K50" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" t="s">
         <v>221</v>
-      </c>
-      <c r="B51" t="s">
-        <v>222</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -2900,22 +2900,22 @@
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F51" t="s">
+        <v>222</v>
+      </c>
+      <c r="G51" t="s">
         <v>223</v>
       </c>
-      <c r="G51" t="s">
-        <v>224</v>
-      </c>
       <c r="H51">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
       </c>
       <c r="K51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2942,13 +2942,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>